<commit_message>
change the sensitvity title
</commit_message>
<xml_diff>
--- a/fig/performance.xlsx
+++ b/fig/performance.xlsx
@@ -2001,7 +2001,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" baseline="0"/>
+              <a:defRPr sz="1200" b="0" baseline="0"/>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -2027,10 +2027,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000"/>
+                  <a:defRPr sz="1200"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1000"/>
+                  <a:rPr lang="en-US" sz="1200"/>
                   <a:t>Memory Usage(MB)</a:t>
                 </a:r>
               </a:p>
@@ -2052,9 +2052,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.903111339563426"/>
-          <c:y val="0.282023549139691"/>
+          <c:y val="0.438273420722978"/>
           <c:w val="0.0803869406226357"/>
-          <c:h val="0.189800962379703"/>
+          <c:h val="0.145585965461704"/>
         </c:manualLayout>
       </c:layout>
       <c:txPr>
@@ -2797,8 +2797,8 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>314960</xdr:colOff>
-      <xdr:row>70</xdr:row>
-      <xdr:rowOff>132080</xdr:rowOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3988,6 +3988,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -4559,6 +4560,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -5363,6 +5365,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -5379,7 +5382,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" view="pageLayout" topLeftCell="C31" zoomScale="125" workbookViewId="0">
+    <sheetView tabSelected="1" showRuler="0" view="pageLayout" topLeftCell="A54" zoomScale="125" workbookViewId="0">
       <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
@@ -6110,6 +6113,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -6318,6 +6322,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>